<commit_message>
Update amplification curves and ddct results with new data
</commit_message>
<xml_diff>
--- a/TN052.13/ddct_results.xlsx
+++ b/TN052.13/ddct_results.xlsx
@@ -1,21 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/nipper_wisc_edu/Documents/qPCR/TN052.13/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_CE75FDCE8F79A8D366075C52F363FA770999D296" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D27BE4E4-A33D-DC40-A5E5-489737E53605}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+  <si>
+    <t>Sample Name</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>DUSP11</t>
+  </si>
+  <si>
+    <t>RNA18S1</t>
+  </si>
+  <si>
+    <t>delta_ct</t>
+  </si>
+  <si>
+    <t>ddct</t>
+  </si>
+  <si>
+    <t>fold_change</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>T0.5</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T1.5</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +116,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +168,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +202,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +237,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,228 +413,195 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sample Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>DUSP11</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>RNA18S1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>delta_ct</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>ddct</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>fold_change</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>T0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>20.07919733333333</v>
       </c>
       <c r="D2">
-        <v>4.4640491</v>
+        <v>4.4640491000000004</v>
       </c>
       <c r="E2">
-        <v>15.61514823333333</v>
+        <v>15.615148233333329</v>
       </c>
       <c r="F2">
         <v>0.1172563111111113</v>
       </c>
       <c r="G2">
-        <v>0.9219393104033866</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>T0</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
+        <v>0.92193931040338661</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3">
         <v>20.08763166666667</v>
       </c>
       <c r="D3">
-        <v>4.6358532</v>
+        <v>4.6358531999999997</v>
       </c>
       <c r="E3">
-        <v>15.45177846666667</v>
+        <v>15.451778466666671</v>
       </c>
       <c r="F3">
-        <v>-0.04611345555555424</v>
+        <v>-4.6113455555554239E-2</v>
       </c>
       <c r="G3">
-        <v>1.032479727940334</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>T0</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
+        <v>1.0324797279403339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>19.85306333333333</v>
+        <v>19.853063333333331</v>
       </c>
       <c r="D4">
-        <v>4.426314266666667</v>
+        <v>4.4263142666666671</v>
       </c>
       <c r="E4">
-        <v>15.42674906666666</v>
+        <v>15.426749066666661</v>
       </c>
       <c r="F4">
-        <v>-0.07114285555555711</v>
+        <v>-7.1142855555557105E-2</v>
       </c>
       <c r="G4">
         <v>1.050548564101254</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>T0.5</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>20.970633</v>
+        <v>20.970632999999999</v>
       </c>
       <c r="D5">
-        <v>5.310584899999999</v>
+        <v>5.3105848999999994</v>
       </c>
       <c r="E5">
-        <v>15.6600481</v>
+        <v>15.660048099999999</v>
       </c>
       <c r="F5">
         <v>0.1621561777777796</v>
       </c>
       <c r="G5">
-        <v>0.8936884116082098</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>T0.5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
+        <v>0.89368841160820978</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>20.231888</v>
+        <v>20.231888000000001</v>
       </c>
       <c r="D6">
-        <v>4.4584274</v>
+        <v>4.4584273999999997</v>
       </c>
       <c r="E6">
         <v>15.7734606</v>
       </c>
       <c r="F6">
-        <v>0.2755686777777804</v>
+        <v>0.27556867777778038</v>
       </c>
       <c r="G6">
-        <v>0.8261246143147278</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>T0.5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
+        <v>0.82612461431472783</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>19.88491</v>
+        <v>19.884910000000001</v>
       </c>
       <c r="D7">
-        <v>4.403471499999999</v>
+        <v>4.4034714999999993</v>
       </c>
       <c r="E7">
-        <v>15.4814385</v>
+        <v>15.481438499999999</v>
       </c>
       <c r="F7">
-        <v>-0.01645342222221835</v>
+        <v>-1.645342222221835E-2</v>
       </c>
       <c r="G7">
         <v>1.011469924099756</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>20.09928766666667</v>
+        <v>20.099287666666669</v>
       </c>
       <c r="D8">
-        <v>4.707475466666667</v>
+        <v>4.7074754666666667</v>
       </c>
       <c r="E8">
         <v>15.3918122</v>
@@ -583,70 +613,58 @@
         <v>1.076299598631445</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>20.024561</v>
+        <v>20.024560999999999</v>
       </c>
       <c r="D9">
-        <v>4.470678833333333</v>
+        <v>4.4706788333333334</v>
       </c>
       <c r="E9">
-        <v>15.55388216666666</v>
+        <v>15.553882166666661</v>
       </c>
       <c r="F9">
-        <v>0.05599024444444289</v>
+        <v>5.5990244444442887E-2</v>
       </c>
       <c r="G9">
-        <v>0.9619339592746804</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
+        <v>0.96193395927468039</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>19.88510966666667</v>
+        <v>19.885109666666668</v>
       </c>
       <c r="D10">
-        <v>4.427190133333333</v>
+        <v>4.4271901333333332</v>
       </c>
       <c r="E10">
-        <v>15.45791953333334</v>
+        <v>15.457919533333341</v>
       </c>
       <c r="F10">
-        <v>-0.0399723888888861</v>
+        <v>-3.9972388888886101E-2</v>
       </c>
       <c r="G10">
         <v>1.02809415022227</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>T1.5</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
       </c>
       <c r="C11">
         <v>20.10237433333333</v>
@@ -658,64 +676,56 @@
         <v>15.40887366666667</v>
       </c>
       <c r="F11">
-        <v>-0.08901825555555476</v>
+        <v>-8.9018255555554759E-2</v>
       </c>
       <c r="G11">
         <v>1.063646131959481</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>T1.5</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
       </c>
       <c r="C12">
         <v>19.96234766666667</v>
       </c>
       <c r="D12">
-        <v>4.437546833333333</v>
+        <v>4.4375468333333332</v>
       </c>
       <c r="E12">
         <v>15.52480083333333</v>
       </c>
       <c r="F12">
-        <v>0.02690891111111249</v>
+        <v>2.6908911111112491E-2</v>
       </c>
       <c r="G12">
-        <v>0.9815210331785341</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>T1.5</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
+        <v>0.98152103317853412</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
       </c>
       <c r="C13">
         <v>20.14031833333333</v>
       </c>
       <c r="D13">
-        <v>4.456004833333333</v>
+        <v>4.4560048333333331</v>
       </c>
       <c r="E13">
         <v>15.6843135</v>
       </c>
       <c r="F13">
-        <v>0.1864215777777787</v>
+        <v>0.18642157777777871</v>
       </c>
       <c r="G13">
-        <v>0.8787827294995186</v>
+        <v>0.87878272949951863</v>
       </c>
     </row>
   </sheetData>

</xml_diff>